<commit_message>
lab104 - naprawiony excel
</commit_message>
<xml_diff>
--- a/Fiz104/Fizyka104.xlsx
+++ b/Fiz104/Fizyka104.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Moje dokumenty\studia\sem 3\sprawka\Fiz104\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\GitHub\Fizyka3.1\Fiz104\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="3" xr2:uid="{8F8CBF2D-9B3C-4C97-8CF8-2FB3F6E6B0FA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{8F8CBF2D-9B3C-4C97-8CF8-2FB3F6E6B0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="ciemna" sheetId="1" r:id="rId1"/>
@@ -8856,7 +8856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4D2850-0402-4621-9B69-365BCFAF9B99}">
   <dimension ref="A1:AB76"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
@@ -13172,7 +13172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4B6E61-CA93-4D83-B654-3567B302F8A5}">
   <dimension ref="A1:BL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+    <sheetView topLeftCell="AE1" workbookViewId="0">
       <selection activeCell="AY3" sqref="AY3:BL6"/>
     </sheetView>
   </sheetViews>

</xml_diff>